<commit_message>
made api changes in staff app
</commit_message>
<xml_diff>
--- a/hms_api's.xlsx
+++ b/hms_api's.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STUDY\hms_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75512F75-E0AA-44CD-917D-488BB4EEABAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D959CE15-58BA-4422-BB2D-F29E1EA21DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>HMS User Registration</t>
   </si>
@@ -138,6 +138,16 @@
   <si>
     <t>[{"doctorid": 1, "name": "Asim Thaha", "username": "asimthaha", "speciality": "Nephrologist", "startYear": 2000,
 "password": "1234", "qualification": "MBBS, MD", "role": "Doctor"}]</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/staff/displayDoctor/</t>
+  </si>
+  <si>
+    <t>HMS All Doctor Display</t>
+  </si>
+  <si>
+    <t>[{"doctorid": 1, "name": "ASIM THAHA AZEEZ", "username": "asimthaha", "speciality": "Nephrologist", "startYear": 2000,
+"qualification": "MBBS, MD", "role": "Doctor", "password": "1234"}]</t>
   </si>
 </sst>
 </file>
@@ -486,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,7 +528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -535,7 +545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -552,7 +562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -569,7 +579,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -586,7 +596,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -603,7 +613,7 @@
         <v>25.393431120317999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -614,7 +624,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -631,7 +641,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -646,6 +656,20 @@
       </c>
       <c r="E9" s="1" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -658,8 +682,9 @@
     <hyperlink ref="C7" r:id="rId6" xr:uid="{B1F594C4-2BDE-4E5C-BA15-34238B17DA10}"/>
     <hyperlink ref="C8" r:id="rId7" xr:uid="{66F7E223-ACA9-4329-83BC-6C0EEEC049ED}"/>
     <hyperlink ref="C9" r:id="rId8" xr:uid="{253DB75C-F161-48B2-8287-F86CC9694D52}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{95152A27-5A38-4B21-90BD-E8AA88C1B240}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made new api for heart disease prediction
</commit_message>
<xml_diff>
--- a/hms_api's.xlsx
+++ b/hms_api's.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STUDY\hms_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D959CE15-58BA-4422-BB2D-F29E1EA21DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5ED5CF-F5FB-4ED0-8572-8A2DA05B0BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>HMS User Registration</t>
   </si>
@@ -148,6 +148,23 @@
   <si>
     <t>[{"doctorid": 1, "name": "ASIM THAHA AZEEZ", "username": "asimthaha", "speciality": "Nephrologist", "startYear": 2000,
 "qualification": "MBBS, MD", "role": "Doctor", "password": "1234"}]</t>
+  </si>
+  <si>
+    <t>HMS Heart Prediction</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/user/predictHeart/</t>
+  </si>
+  <si>
+    <t>{"age":45,"sex":1,"cp":1,"trestbps":145,"chol":220,"fbs":1,"restecg":2,"thalach":150,"exang":1, "oldpeak":2.34,"slope":3,"ca":3.2, "thal":5.0}</t>
+  </si>
+  <si>
+    <t>{"result": "The person does not have a Heart Disease", "tips": ["Maintain a balanced diet with fruits, vegetables, lean
+proteins, and healthy fats.", "Stay physically active to maintain a healthy weight and cardiovascular fitness.", "Avoid
+smoking and seek help to quit if needed.", "Limit alcohol consumption to moderate levels.", "Practice stress-relief
+techniques to reduce the impact of stress.", "Schedule regular health check-ups for early detection and prevention."],
+"youtube_links": {"heart_disease_management": "https://www.youtube.com/watch?v=IMBpwpf5crU", "heart_disease_prevention":
+"https://www.youtube.com/watch?v=B6UYNZLpAMs"}}</t>
   </si>
 </sst>
 </file>
@@ -496,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,6 +689,23 @@
         <v>38</v>
       </c>
     </row>
+    <row r="11" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{3DE50634-016E-4C3E-8A85-EB6310316EBC}"/>
@@ -683,8 +717,9 @@
     <hyperlink ref="C8" r:id="rId7" xr:uid="{66F7E223-ACA9-4329-83BC-6C0EEEC049ED}"/>
     <hyperlink ref="C9" r:id="rId8" xr:uid="{253DB75C-F161-48B2-8287-F86CC9694D52}"/>
     <hyperlink ref="C10" r:id="rId9" xr:uid="{95152A27-5A38-4B21-90BD-E8AA88C1B240}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{61BAEE91-CE44-482A-A78D-E9225772D2EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made a new model for result
</commit_message>
<xml_diff>
--- a/hms_api's.xlsx
+++ b/hms_api's.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STUDY\hms_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2229431B-C6FB-4FE7-865C-ECC542758EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92F5543-201D-405A-84F8-DEB5516B8B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>HMS User Registration</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>{"bookingid":1, "userid":1,"doctorid":2, "time":"11:30", "date": "24/12/2023"}</t>
+  </si>
+  <si>
+    <t>{"status": "Appoinment Successful"}</t>
   </si>
 </sst>
 </file>
@@ -518,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,7 +644,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -647,6 +653,12 @@
       </c>
       <c r="C7" s="3" t="s">
         <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="144" x14ac:dyDescent="0.3">

</xml_diff>